<commit_message>
cambio final falta cambiar las hojas de cambio climatico
</commit_message>
<xml_diff>
--- a/docs/xlsx/Matriz_IGA.xlsx
+++ b/docs/xlsx/Matriz_IGA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AGIEN\Documents\GGC-0805-2025\Politica y Relacionamiento Ambiental\Indicador de gobernaza\INDICE DE GOBERNANZA SME 2023\IGA\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC0BC61-FF1C-4EF6-8891-4278A373F39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A9840-BB30-46F0-9920-1AB1743263E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{05641854-7AD6-4C4A-B363-B2374F45EEBE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{05641854-7AD6-4C4A-B363-B2374F45EEBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable_indicador" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
   <calcPr calcId="191029" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6132,16 +6132,10 @@
   </cellStyles>
   <dxfs count="37">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -6185,6 +6179,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -6202,6 +6199,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -8402,132 +8402,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CBDBB2ED-8600-4915-BB56-BAD06FC59A86}" name="TablaDinámica3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A29:C48" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="19">
-        <item x="9"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="6"/>
-        <item x="0"/>
-        <item x="14"/>
-        <item x="4"/>
-        <item x="17"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="10"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="19">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Suma de Puntaje para la gobernanza" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Suma de Puntaje máximo del indicador" fld="7" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{264A6054-B8D0-49F1-958F-4CC79973A187}" name="TablaDinámica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{264A6054-B8D0-49F1-958F-4CC79973A187}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A21:C26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -8595,7 +8470,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A10DDEA5-2ED5-44C1-AE1A-4D6FF91D4B53}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
@@ -8725,8 +8600,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6301C740-09EA-48FB-B0E3-9F0B578B7B3C}" name="TablaDinámica17" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6301C740-09EA-48FB-B0E3-9F0B578B7B3C}" name="TablaDinámica17" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A50:B113" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -9022,8 +8897,133 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CBDBB2ED-8600-4915-BB56-BAD06FC59A86}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A29:C48" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="19">
+        <item x="9"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="4"/>
+        <item x="17"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Suma de Puntaje para la gobernanza" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Suma de Puntaje máximo del indicador" fld="7" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94F753B4-D13A-40E3-A635-BA173337E7D2}" name="TablaDinámica3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94F753B4-D13A-40E3-A635-BA173337E7D2}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A29:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -9139,11 +9139,26 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BCE37292-0E4A-4B18-A241-FF01A22DF8EE}" name="TablaDinámica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A19:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BCE37292-0E4A-4B18-A241-FF01A22DF8EE}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A19:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="12">
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="7"/>
+        <item h="1" x="4"/>
+        <item h="1" x="2"/>
+        <item h="1" x="10"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="2"/>
@@ -9163,18 +9178,12 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -9183,6 +9192,9 @@
   <colItems count="1">
     <i/>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Promedio de Porcentaje alcanzado" fld="8" subtotal="average" baseField="2" baseItem="0" numFmtId="1"/>
   </dataFields>
@@ -9199,7 +9211,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87A1B2CB-2C7A-41FC-8942-4F746F312DC8}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{87A1B2CB-2C7A-41FC-8942-4F746F312DC8}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -9275,7 +9287,7 @@
     <dataField name="Promedio de Porcentaje alcanzado" fld="8" subtotal="average" baseField="1" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -9366,11 +9378,11 @@
     <tableColumn id="4" xr3:uid="{C4432B99-A6AE-48F9-BD0D-8A209C21B04D}" name="Atributo" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{A1B26168-A432-4C82-9EAB-550809B6A394}" name="Índice / Indicador" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{27CFA83E-C610-4A84-AA98-41781D762475}" name="Resultado del indicador _x000a_(en sus unidades)" dataDxfId="7" dataCellStyle="Porcentaje"/>
-    <tableColumn id="7" xr3:uid="{B6AD0A31-B2EC-443A-98FF-B8723066A05A}" name="Puntaje para la gobernanza" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{48555891-5B3A-4346-A51B-D77BF5507381}" name="Puntaje máximo del indicador" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="1">
+    <tableColumn id="7" xr3:uid="{B6AD0A31-B2EC-443A-98FF-B8723066A05A}" name="Puntaje para la gobernanza" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{48555891-5B3A-4346-A51B-D77BF5507381}" name="Puntaje máximo del indicador" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3">
       <calculatedColumnFormula>Tabla1[[#This Row],[Aproximación a la unidad]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{DEE1B35F-D35D-4BA8-BFAE-03EFE4827BAD}" name="Porcentaje alcanzado" totalsRowFunction="average" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="9" xr3:uid="{DEE1B35F-D35D-4BA8-BFAE-03EFE4827BAD}" name="Porcentaje alcanzado" totalsRowFunction="average" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>G2/H2*100</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{2FD814FE-9E97-4024-8889-C71BA29A07EA}" name="Columna1"/>
@@ -57518,8 +57530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BEDCC86-3FB7-4809-9E7F-438575BD5A3D}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59294,13 +59306,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D58B37-A53D-46D5-9326-D9679D4AF825}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
   </cols>
@@ -59457,6 +59469,14 @@
         <v>57.20228930299956</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="48" t="s">
         <v>283</v>
@@ -59470,7 +59490,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="31">
-        <v>68.740991234066044</v>
+        <v>60.526315789473685</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -59478,31 +59498,15 @@
         <v>125</v>
       </c>
       <c r="B21" s="31">
-        <v>53.015301814505698</v>
+        <v>10.526315789473683</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
-        <v>155</v>
+        <v>284</v>
       </c>
       <c r="B22" s="31">
-        <v>51.078745815587922</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="31">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="49" t="s">
-        <v>284</v>
-      </c>
-      <c r="B24" s="31">
-        <v>57.20228930299956</v>
+        <v>43.859649122807014</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>